<commit_message>
Adding number from 5 to 10
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\Git_Projects\TestRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9030AE58-1ADB-4789-A191-C9553444BA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31AC08B-6234-4AC0-A035-A3F668CE2FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,10 +345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,6 +383,31 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
remove number from 10 to 8
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\Git_Projects\TestRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31AC08B-6234-4AC0-A035-A3F668CE2FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8FBD78-A14F-4FB9-B9C0-78638B0C1E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,10 +345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A10" sqref="A10:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,16 +398,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>